<commit_message>
Se agregan datos al xls
</commit_message>
<xml_diff>
--- a/Exercise/Datos Complementarios.xlsx
+++ b/Exercise/Datos Complementarios.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4051\Datos\ProyectoBgD\AutomaticLearning\Exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97123CF-3C49-447A-9C03-ABD71AB4CECC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A87C5D7-D3CB-49CA-8597-E13175758F7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{7D0B0809-8ABD-4AD6-8C9F-9DB6D01E9F90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{7D0B0809-8ABD-4AD6-8C9F-9DB6D01E9F90}"/>
   </bookViews>
   <sheets>
     <sheet name="Dimensiones-Variables" sheetId="2" r:id="rId1"/>
     <sheet name="Plan de Trabajo" sheetId="3" r:id="rId2"/>
     <sheet name="Propuesta - Tabla" sheetId="4" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Dimensiones-Variables'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Propuesta - Tabla'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="115">
   <si>
     <r>
       <t>1.</t>
@@ -487,9 +489,6 @@
     <t>placeID</t>
   </si>
   <si>
-    <t>Numerico</t>
-  </si>
-  <si>
     <t>Comentarios</t>
   </si>
   <si>
@@ -514,18 +513,6 @@
     <t>chefmozaccepts.csv</t>
   </si>
   <si>
-    <t>Otros medios de pagos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> chefmozcuisine.csv</t>
-  </si>
-  <si>
-    <t>Se analizará el archivo usercuisine.csv para determinar las categorias que en la distribucion de clientes abarque las clases relevantes</t>
-  </si>
-  <si>
-    <t>&lt;&lt;Analizar&gt;&gt;</t>
-  </si>
-  <si>
     <t>chefmozhours4.csv</t>
   </si>
   <si>
@@ -548,13 +535,277 @@
   </si>
   <si>
     <t>Se considera como parking los valores(yes,valet_parking, free, validated_parking)</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>Rpayment</t>
+  </si>
+  <si>
+    <t>Rcuisine</t>
+  </si>
+  <si>
+    <t>parking_lot</t>
+  </si>
+  <si>
+    <t>geoplaces2.csv</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vamos a seleccionar solo los siguientes medios de pagos que tienen la tabla de clientes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(userpayment.csv)</t>
+    </r>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>Codigo Postal</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitud</t>
+  </si>
+  <si>
+    <t>longitud</t>
+  </si>
+  <si>
+    <t>alcohol</t>
+  </si>
+  <si>
+    <t>smoking_area</t>
+  </si>
+  <si>
+    <t>dress_code</t>
+  </si>
+  <si>
+    <t>vestimenta</t>
+  </si>
+  <si>
+    <t>Fumadores?</t>
+  </si>
+  <si>
+    <t>accessibility</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Rambience</t>
+  </si>
+  <si>
+    <t>franchise</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>other_services</t>
+  </si>
+  <si>
+    <t>¿internet?</t>
+  </si>
+  <si>
+    <t>Acceso?</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>franquicia</t>
+  </si>
+  <si>
+    <t>area_abierto_cerrado</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>food_rating</t>
+  </si>
+  <si>
+    <t>service_rating</t>
+  </si>
+  <si>
+    <t>Numeric</t>
+  </si>
+  <si>
+    <t>3 [0,1,2]</t>
+  </si>
+  <si>
+    <t>rating_final.csv</t>
+  </si>
+  <si>
+    <t>ambiente</t>
+  </si>
+  <si>
+    <t>Nominal</t>
+  </si>
+  <si>
+    <t>Transformación de datos</t>
+  </si>
+  <si>
+    <t>Valores unicos</t>
+  </si>
+  <si>
+    <t>3 [No_Alcohol_Served,Wine_Beer,Full_Bar]</t>
+  </si>
+  <si>
+    <t>none,only_at_bar,permitted,section,not_permitted</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Este valor es positivo cuando: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>only_at_bar/permitted / section</t>
+    </r>
+  </si>
+  <si>
+    <t>informal,casual,formal</t>
+  </si>
+  <si>
+    <t>no_accessibility,completely,partially</t>
+  </si>
+  <si>
+    <t>medium,low,high</t>
+  </si>
+  <si>
+    <t>familiar,quiet</t>
+  </si>
+  <si>
+    <t>t,f</t>
+  </si>
+  <si>
+    <t>open,closed</t>
+  </si>
+  <si>
+    <t>[none,internet,variety]</t>
+  </si>
+  <si>
+    <t>Descartamos este valor porque no es representativo para la muestra de datos</t>
+  </si>
+  <si>
+    <t>[Afghan,African,American,Armenian,Asian,Bagels,Bakery,Bar,Bar_Pub_Brewery,Barbecue,Brazilian,Breakfast-Brunch,Burgers,Cafe-Coffee_Shop,</t>
+  </si>
+  <si>
+    <t>Cafeteria,California,Caribbean,Chinese,Contemporary,Continental-European,Deli-Sandwiches,Dessert-Ice_Cream,Diner,Dutch-Belgian,Eastern_European,Ethiopian,Family,Fast_Food,Fine_Dining,French,,Game,German,Greek,Hot_Dogs,</t>
+  </si>
+  <si>
+    <t>International,Italian,Japanese,Juice,Korean,Latin_American,Mediterranean,Mexican,Mongolian,Organic-Healthy,Persian,</t>
+  </si>
+  <si>
+    <t>Pizzeria,Polish,Regional,Seafood,Soup,Southern,Southwestern,Spanish,Steaks,Sushi,Thai,Turkish,Vegetarian,Vietnamese]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">VISA  == YES </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cuando</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Rpayment = VISA</t>
+    </r>
+  </si>
+  <si>
+    <t>MasterCard-Eurocard == YES cuando Rpayment = MasterCard-Eurocard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bank_debit_cards == YES cuando Rpayment = bank_debit_cards </t>
+  </si>
+  <si>
+    <t>cash == YES cuando Rpayment = cash</t>
+  </si>
+  <si>
+    <t>American_Express  == YES cuando Rpayment=  American_Express</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Tipo de comida</t>
+  </si>
+  <si>
+    <t>parking_lot = yes,valet_parking, free, validated_parking</t>
+  </si>
+  <si>
+    <t>public,none,yes,valet_parking,free,street,validated_parking]</t>
+  </si>
+  <si>
+    <t>Realizar transformaciones de datos</t>
+  </si>
+  <si>
+    <t>cash
+VISA
+MasterCard-Eurocard
+American_Express
+bank_debit_cards
+checks
+Discover
+Carte_Blanche
+Diners_Club
+Visa
+Japan_Credit_Bureau
+gift_certificates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,6 +822,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -611,17 +878,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -959,7 +1235,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -967,31 +1243,31 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -999,43 +1275,43 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1043,31 +1319,31 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="3"/>
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1125,177 +1401,1091 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4449A61E-5FDC-4CA2-B3A1-C9C247C4E39C}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="4"/>
+    <col min="1" max="1" width="28.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.42578125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G6" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="B12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="G12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>51</v>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G1" xr:uid="{03D56B1A-AD50-449F-BF58-2F62D1A108F9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C026F94-E21D-4A94-8396-07447C8DEB1D}">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection sqref="A1:F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se actualiza las variables con ETL
</commit_message>
<xml_diff>
--- a/Exercise/Datos Complementarios.xlsx
+++ b/Exercise/Datos Complementarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4051\Datos\ProyectoBgD\AutomaticLearning\Exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A87C5D7-D3CB-49CA-8597-E13175758F7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92AAD61-EFC3-488A-90EF-4AA130916F14}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{7D0B0809-8ABD-4AD6-8C9F-9DB6D01E9F90}"/>
   </bookViews>
@@ -16,9 +16,10 @@
     <sheet name="Dimensiones-Variables" sheetId="2" r:id="rId1"/>
     <sheet name="Plan de Trabajo" sheetId="3" r:id="rId2"/>
     <sheet name="Propuesta - Tabla" sheetId="4" r:id="rId3"/>
-    <sheet name="Hoja1" sheetId="5" r:id="rId4"/>
+    <sheet name="Datos Reales" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Datos Reales'!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Dimensiones-Variables'!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Propuesta - Tabla'!$A$1:$G$1</definedName>
   </definedNames>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="125">
   <si>
     <r>
       <t>1.</t>
@@ -799,6 +800,36 @@
 Visa
 Japan_Credit_Bureau
 gift_certificates</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Cantidad de medios de pagos</t>
+  </si>
+  <si>
+    <t>Numerico</t>
+  </si>
+  <si>
+    <t>Contar la cantidad de medios de pagos aceptados</t>
+  </si>
+  <si>
+    <t>Cantidad de tipos de comida</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>longitud y longitud para calculo de distancia entre restaurantes</t>
+  </si>
+  <si>
+    <t>distancias</t>
+  </si>
+  <si>
+    <t>boleano</t>
   </si>
 </sst>
 </file>
@@ -878,14 +909,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -898,6 +926,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1235,7 +1275,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1243,31 +1283,31 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1275,43 +1315,43 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1319,31 +1359,31 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1404,559 +1444,559 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.42578125" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="5"/>
+    <col min="1" max="1" width="28.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.42578125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M11" s="4" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1969,523 +2009,393 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C026F94-E21D-4A94-8396-07447C8DEB1D}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection sqref="A1:F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="F15" s="4"/>
+      <c r="G15" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="F18" s="4"/>
+      <c r="G18" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4"/>
+      <c r="G19" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F29" s="5"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:G1" xr:uid="{4C3043D7-C7D7-46FB-AA03-FD2A396C4C36}">
+    <sortState ref="A2:G19">
+      <sortCondition ref="F1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se atualizan las variables
</commit_message>
<xml_diff>
--- a/Exercise/Datos Complementarios.xlsx
+++ b/Exercise/Datos Complementarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4051\Datos\ProyectoBgD\AutomaticLearning\Exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92AAD61-EFC3-488A-90EF-4AA130916F14}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E9A5B8-BB8E-4EF4-9332-084040C29A40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{7D0B0809-8ABD-4AD6-8C9F-9DB6D01E9F90}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="125">
   <si>
     <r>
       <t>1.</t>
@@ -927,9 +927,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -938,6 +935,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1275,7 +1275,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1283,31 +1283,31 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1315,43 +1315,43 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1359,31 +1359,31 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -2013,12 +2013,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="9" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" customWidth="1"/>
@@ -2028,7 +2028,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -2070,7 +2070,7 @@
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>110</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2089,7 +2089,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -2112,7 +2112,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2131,7 +2131,7 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>66</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -2150,7 +2150,7 @@
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>75</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2169,7 +2169,7 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -2188,7 +2188,7 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>85</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2207,7 +2207,7 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>77</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -2226,7 +2226,7 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>78</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2245,7 +2245,7 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>80</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2264,7 +2264,7 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>79</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -2283,7 +2283,7 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>81</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -2302,7 +2302,7 @@
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>117</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -2321,7 +2321,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>120</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2334,7 +2334,7 @@
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -2353,7 +2353,7 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>123</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -2366,13 +2366,15 @@
       <c r="E18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="G18" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="4" t="s">

</xml_diff>

<commit_message>
Actualiacion del archivo con las variables cargadas
</commit_message>
<xml_diff>
--- a/Exercise/Datos Complementarios.xlsx
+++ b/Exercise/Datos Complementarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4051\Datos\ProyectoBgD\AutomaticLearning\Exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E9A5B8-BB8E-4EF4-9332-084040C29A40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A40E12-BB4E-4558-989F-391389BCD87A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{7D0B0809-8ABD-4AD6-8C9F-9DB6D01E9F90}"/>
   </bookViews>
@@ -2013,7 +2013,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Actualización del perfil de datos
</commit_message>
<xml_diff>
--- a/Exercise/Datos Complementarios.xlsx
+++ b/Exercise/Datos Complementarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4051\Datos\ProyectoBgD\AutomaticLearning\Exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A40E12-BB4E-4558-989F-391389BCD87A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68E899D-8A2F-4891-8130-692A3B6E2177}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{7D0B0809-8ABD-4AD6-8C9F-9DB6D01E9F90}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="126">
   <si>
     <r>
       <t>1.</t>
@@ -830,6 +830,9 @@
   </si>
   <si>
     <t>boleano</t>
+  </si>
+  <si>
+    <t>isSmoking</t>
   </si>
 </sst>
 </file>
@@ -2012,8 +2015,8 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,7 +2378,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>124</v>
@@ -2387,7 +2390,9 @@
       <c r="E19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="G19" s="4" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Se actualiza con la info del modelo, codo y silueta
</commit_message>
<xml_diff>
--- a/Exercise/Datos Complementarios.xlsx
+++ b/Exercise/Datos Complementarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4051\Datos\ProyectoBgD\AutomaticLearning\Exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68E899D-8A2F-4891-8130-692A3B6E2177}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A331ABD6-0C74-40A7-9430-F13226603419}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{7D0B0809-8ABD-4AD6-8C9F-9DB6D01E9F90}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Datos Reales" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Datos Reales'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Datos Reales'!$A$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Dimensiones-Variables'!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Propuesta - Tabla'!$A$1:$G$1</definedName>
   </definedNames>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="140">
   <si>
     <r>
       <t>1.</t>
@@ -826,20 +826,62 @@
     <t>longitud y longitud para calculo de distancia entre restaurantes</t>
   </si>
   <si>
-    <t>distancias</t>
-  </si>
-  <si>
     <t>boleano</t>
   </si>
   <si>
     <t>isSmoking</t>
+  </si>
+  <si>
+    <t>Distancia Punto 1</t>
+  </si>
+  <si>
+    <t>Distancia Punto 2</t>
+  </si>
+  <si>
+    <t>Distancia Punto 3</t>
+  </si>
+  <si>
+    <t>Grupo de ciudad</t>
+  </si>
+  <si>
+    <t>Nombre Proyecto</t>
+  </si>
+  <si>
+    <t>distPoint1</t>
+  </si>
+  <si>
+    <t>distPoint2</t>
+  </si>
+  <si>
+    <t>distPoint3</t>
+  </si>
+  <si>
+    <t>classCity</t>
+  </si>
+  <si>
+    <t>¿Permite fumadores?</t>
+  </si>
+  <si>
+    <t>foodCount</t>
+  </si>
+  <si>
+    <t>Tipos de medios de pagos</t>
+  </si>
+  <si>
+    <t>Tipos de areas para fumadores</t>
+  </si>
+  <si>
+    <t>foodRating</t>
+  </si>
+  <si>
+    <t>serviceRating</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -875,6 +917,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -912,7 +967,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -930,17 +985,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1278,7 +1334,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1286,31 +1342,31 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1318,43 +1374,43 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1362,31 +1418,31 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -2012,397 +2068,498 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C026F94-E21D-4A94-8396-07447C8DEB1D}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="C4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="H4" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="C6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="C7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="C8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="C9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="C10" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="C11" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="C16" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="C18" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" s="4" t="s">
+      <c r="H18" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="H22" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="C23" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>91</v>
+      <c r="D23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{4C3043D7-C7D7-46FB-AA03-FD2A396C4C36}">
-    <sortState ref="A2:G19">
-      <sortCondition ref="F1"/>
+  <autoFilter ref="A1:H1" xr:uid="{4C3043D7-C7D7-46FB-AA03-FD2A396C4C36}">
+    <sortState ref="A2:H22">
+      <sortCondition ref="G1"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
con cambio de variable cuisine
</commit_message>
<xml_diff>
--- a/Exercise/Datos Complementarios.xlsx
+++ b/Exercise/Datos Complementarios.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4051\Datos\ProyectoBgD\AutomaticLearning\Exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leticia\Documents\R\AutomaticLearning\Exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC381F0-D9A0-43F6-A008-6543511D355E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Dimensiones-Variables" sheetId="2" r:id="rId1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="166">
   <si>
     <r>
       <t>1.</t>
@@ -731,9 +730,6 @@
     <t xml:space="preserve">Se crea una nueva variable con la cantidad de tipos de comida ofrecidos </t>
   </si>
   <si>
-    <t>Con esta transformación se corrige el problema de restaurantes con mas de un tipo de comidas sin perder información.</t>
-  </si>
-  <si>
     <t>Parking_lot</t>
   </si>
   <si>
@@ -879,12 +875,24 @@
   </si>
   <si>
     <t>Establece si el local cuenta con área para fumadores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una vez corridos los modelos detectamos que todos los registros que quedan con un valor por defecto por no estar presentes quedaban clusterizados en el mismo grupo cuando en realidad eran un valor sin información. </t>
+  </si>
+  <si>
+    <t>TypeCuisine</t>
+  </si>
+  <si>
+    <t>American, Asian, Bar, Café-Breakfast, Europea, Fast_Food, International, Mexican, Others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se crea una nueva variable con las clases agrupadas </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1299,7 +1307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1375,12 +1383,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1411,6 +1413,21 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1459,6 +1476,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1772,7 +1799,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1795,7 +1822,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="50" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1803,31 +1830,31 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
+      <c r="A3" s="50"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="50" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1835,43 +1862,43 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="50" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1879,37 +1906,37 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:B1">
     <sortState ref="A2:B19">
       <sortCondition ref="A1"/>
     </sortState>
@@ -1925,10 +1952,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52927AD3-3C67-4AEA-9031-2C74803122B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
@@ -1942,181 +1969,181 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="46" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="44" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="52"/>
+      <c r="B3" s="42" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49"/>
-      <c r="B3" s="44" t="s">
+      <c r="C3" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="44" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="52"/>
+      <c r="B4" s="42" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49"/>
-      <c r="B4" s="44" t="s">
+      <c r="C4" s="42"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="52"/>
+      <c r="B5" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="44"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
-      <c r="B5" s="44" t="s">
+      <c r="C5" s="42"/>
+    </row>
+    <row r="6" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="53"/>
+      <c r="B6" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="44"/>
-    </row>
-    <row r="6" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="43" t="s">
+      <c r="C6" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="C6" s="44" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="54" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="51" t="s">
+      <c r="B7" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="C7" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="43" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="52"/>
+      <c r="B8" s="41" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
-      <c r="B8" s="43" t="s">
+      <c r="C8" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="C8" s="43" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="52"/>
+      <c r="B9" s="41" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="43" t="s">
+      <c r="C9" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="C9" s="43" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="52"/>
+      <c r="B10" s="41" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
-      <c r="B10" s="43" t="s">
+      <c r="C10" s="41"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="52"/>
+      <c r="B11" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="43"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
-      <c r="B11" s="43" t="s">
+      <c r="C11" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="C11" s="43" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="52"/>
+      <c r="B12" s="41" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
-      <c r="B12" s="43" t="s">
+      <c r="C12" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="C12" s="43" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="52"/>
+      <c r="B13" s="41" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="43" t="s">
+      <c r="C13" s="41" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="52"/>
+      <c r="B14" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="C13" s="43" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
-      <c r="B14" s="43" t="s">
+      <c r="C14" s="41"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="53"/>
+      <c r="B15" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="C14" s="43"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
-      <c r="B15" s="43" t="s">
+      <c r="C15" s="41"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="43"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="43" t="s">
+      <c r="C16" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="43" t="s">
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="52"/>
+      <c r="B17" s="41" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
-      <c r="B17" s="43" t="s">
+      <c r="C17" s="41"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="52"/>
+      <c r="B18" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="C17" s="43"/>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
-      <c r="B18" s="43" t="s">
+      <c r="C18" s="41"/>
+    </row>
+    <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="52"/>
+      <c r="B19" s="41" t="s">
         <v>158</v>
       </c>
-      <c r="C18" s="43"/>
-    </row>
-    <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="43" t="s">
+      <c r="C19" s="41"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="52"/>
+      <c r="B20" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="C19" s="43"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
-      <c r="B20" s="43" t="s">
+      <c r="C20" s="41"/>
+    </row>
+    <row r="21" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="53"/>
+      <c r="B21" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="C20" s="43"/>
-    </row>
-    <row r="21" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50"/>
-      <c r="B21" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="C21" s="43"/>
+      <c r="C21" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2130,7 +2157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2148,30 +2175,30 @@
       <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52" t="s">
+      <c r="D2" s="55"/>
+      <c r="E2" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52" t="s">
+      <c r="F2" s="55"/>
+      <c r="G2" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52" t="s">
+      <c r="H2" s="55"/>
+      <c r="I2" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52" t="s">
+      <c r="J2" s="55"/>
+      <c r="K2" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52" t="s">
+      <c r="L2" s="55"/>
+      <c r="M2" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="53"/>
+      <c r="N2" s="56"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
@@ -2289,12 +2316,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,18 +2339,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="58" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -2361,7 +2388,7 @@
       <c r="B3" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D3" s="20"/>
@@ -2371,7 +2398,7 @@
       <c r="F3" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="35" t="s">
         <v>97</v>
       </c>
       <c r="H3" s="20" t="s">
@@ -2381,28 +2408,28 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F4" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="40" t="s">
         <v>97</v>
       </c>
       <c r="H4" s="23"/>
-      <c r="I4" s="38"/>
+      <c r="I4" s="36"/>
     </row>
     <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
@@ -2426,10 +2453,10 @@
       <c r="G5" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="H5" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="I5" s="60" t="s">
+      <c r="I5" s="63" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2455,8 +2482,8 @@
       <c r="G6" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H6" s="55"/>
-      <c r="I6" s="61"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="64"/>
     </row>
     <row r="7" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
@@ -2480,8 +2507,8 @@
       <c r="G7" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="55"/>
-      <c r="I7" s="61"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="64"/>
     </row>
     <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -2629,31 +2656,31 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="33" t="s">
+      <c r="B13" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="36" t="s">
+      <c r="G13" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="I13" s="35"/>
+      <c r="I13" s="67"/>
     </row>
     <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -2662,8 +2689,8 @@
       <c r="B14" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="28" t="s">
-        <v>127</v>
+      <c r="C14" s="45" t="s">
+        <v>126</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>100</v>
@@ -2677,11 +2704,11 @@
       <c r="G14" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="I14" s="18" t="s">
-        <v>113</v>
+      <c r="I14" s="47" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -2691,8 +2718,8 @@
       <c r="B15" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="28" t="s">
-        <v>127</v>
+      <c r="C15" s="46" t="s">
+        <v>126</v>
       </c>
       <c r="D15" s="25" t="s">
         <v>100</v>
@@ -2706,11 +2733,11 @@
       <c r="G15" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H15" s="28" t="s">
+      <c r="H15" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="I15" s="32" t="s">
-        <v>113</v>
+      <c r="I15" s="48" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -2720,8 +2747,8 @@
       <c r="B16" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="28" t="s">
-        <v>127</v>
+      <c r="C16" s="46" t="s">
+        <v>126</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>100</v>
@@ -2735,11 +2762,11 @@
       <c r="G16" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="I16" s="32" t="s">
-        <v>113</v>
+      <c r="I16" s="48" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -2749,8 +2776,8 @@
       <c r="B17" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="28" t="s">
-        <v>127</v>
+      <c r="C17" s="46" t="s">
+        <v>126</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>100</v>
@@ -2764,11 +2791,11 @@
       <c r="G17" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H17" s="28" t="s">
+      <c r="H17" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="I17" s="32" t="s">
-        <v>113</v>
+      <c r="I17" s="48" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -2778,8 +2805,8 @@
       <c r="B18" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="28" t="s">
-        <v>127</v>
+      <c r="C18" s="46" t="s">
+        <v>126</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>100</v>
@@ -2793,11 +2820,11 @@
       <c r="G18" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="28" t="s">
+      <c r="H18" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="I18" s="32" t="s">
-        <v>113</v>
+      <c r="I18" s="48" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -2807,8 +2834,8 @@
       <c r="B19" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="28" t="s">
-        <v>127</v>
+      <c r="C19" s="46" t="s">
+        <v>126</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>100</v>
@@ -2822,11 +2849,11 @@
       <c r="G19" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="I19" s="32" t="s">
-        <v>113</v>
+      <c r="I19" s="48" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -2836,8 +2863,8 @@
       <c r="B20" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="28" t="s">
-        <v>127</v>
+      <c r="C20" s="46" t="s">
+        <v>126</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>100</v>
@@ -2851,11 +2878,11 @@
       <c r="G20" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="I20" s="32" t="s">
-        <v>113</v>
+      <c r="I20" s="48" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -2865,8 +2892,8 @@
       <c r="B21" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="28" t="s">
-        <v>127</v>
+      <c r="C21" s="46" t="s">
+        <v>126</v>
       </c>
       <c r="D21" s="25" t="s">
         <v>100</v>
@@ -2880,11 +2907,11 @@
       <c r="G21" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="28" t="s">
+      <c r="H21" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="I21" s="32" t="s">
-        <v>113</v>
+      <c r="I21" s="48" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -2894,8 +2921,8 @@
       <c r="B22" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="28" t="s">
-        <v>127</v>
+      <c r="C22" s="46" t="s">
+        <v>126</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>100</v>
@@ -2909,124 +2936,122 @@
       <c r="G22" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="28" t="s">
+      <c r="H22" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="I22" s="32" t="s">
+      <c r="I22" s="48" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="66"/>
+      <c r="H23" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="I23" s="48"/>
+    </row>
+    <row r="24" spans="1:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="H24" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="I24" s="34"/>
+    </row>
+    <row r="25" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="24" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="28" t="s">
+      <c r="B25" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="D23" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="F23" s="27" t="s">
+      <c r="D25" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="I25" s="48"/>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="36" t="s">
+      <c r="C26" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="H23" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="I23" s="34"/>
-    </row>
-    <row r="24" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="F24" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="H24" s="30" t="s">
+      <c r="H26" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="I24" s="18"/>
-    </row>
-    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="H25" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="I25" s="40"/>
-    </row>
-    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="I26" s="38"/>
+    </row>
+    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
         <v>48</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="H26" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="I26" s="41"/>
-    </row>
-    <row r="27" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
-        <v>50</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>51</v>
@@ -3038,7 +3063,7 @@
         <v>53</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F27" s="29" t="s">
         <v>51</v>
@@ -3047,283 +3072,283 @@
         <v>97</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="I27" s="41"/>
-    </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="I27" s="39"/>
+    </row>
+    <row r="28" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="I28" s="39"/>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" s="23" t="s">
+      <c r="B29" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E29" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="H28" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="I28" s="18"/>
-    </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="F29" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="F29" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="G29" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="H29" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="I29" s="32"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
-        <v>41</v>
-      </c>
       <c r="B30" s="25" t="s">
         <v>54</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E30" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="I30" s="32"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="28" t="s">
+      <c r="B31" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="H30" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="I30" s="32"/>
-    </row>
-    <row r="31" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>58</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E31" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="I31" s="32"/>
+    </row>
+    <row r="32" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" s="28" t="s">
+      <c r="B32" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="28" t="s">
         <v>58</v>
-      </c>
-      <c r="H31" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="I31" s="32"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>59</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F32" s="29" t="s">
         <v>54</v>
       </c>
       <c r="G32" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H32" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I32" s="32"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="25" t="s">
         <v>54</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E33" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="H33" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="I33" s="32"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G33" s="28" t="s">
+      <c r="B34" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="28" t="s">
         <v>60</v>
-      </c>
-      <c r="H33" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="I33" s="32"/>
-    </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>61</v>
       </c>
       <c r="D34" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E34" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G34" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="I34" s="32"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="29"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="I34" s="32" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
-        <v>46</v>
-      </c>
       <c r="B35" s="25" t="s">
         <v>54</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E35" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="29"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I35" s="32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G35" s="28" t="s">
+      <c r="B36" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="28" t="s">
         <v>62</v>
-      </c>
-      <c r="H35" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="I35" s="32"/>
-    </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="28" t="s">
-        <v>120</v>
       </c>
       <c r="D36" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E36" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="H36" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="I36" s="32"/>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="F36" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G36" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="H36" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="I36" s="32" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
-        <v>125</v>
-      </c>
       <c r="B37" s="25" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="F37" s="25" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="G37" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="H37" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="I37" s="32"/>
+        <v>119</v>
+      </c>
+      <c r="H37" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="I37" s="32" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="38" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B38" s="25" t="s">
         <v>51</v>
@@ -3335,7 +3360,7 @@
         <v>38</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F38" s="25" t="s">
         <v>51</v>
@@ -3343,12 +3368,14 @@
       <c r="G38" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="H38" s="55"/>
+      <c r="H38" s="58" t="s">
+        <v>125</v>
+      </c>
       <c r="I38" s="32"/>
     </row>
     <row r="39" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B39" s="25" t="s">
         <v>51</v>
@@ -3360,7 +3387,7 @@
         <v>38</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F39" s="25" t="s">
         <v>51</v>
@@ -3368,44 +3395,58 @@
       <c r="G39" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="55"/>
+      <c r="H39" s="58"/>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="B40" s="27" t="s">
+    <row r="40" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="33" t="s">
+      <c r="C40" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="D40" s="27" t="s">
+      <c r="D40" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="27" t="s">
+      <c r="E40" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G40" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="H40" s="58"/>
+      <c r="I40" s="32"/>
+    </row>
+    <row r="41" spans="1:9" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="27" t="s">
+      <c r="F41" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="G40" s="33" t="s">
+      <c r="G41" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="H40" s="62"/>
-      <c r="I40" s="34"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="32"/>
+      <c r="H41" s="65"/>
+      <c r="I41" s="34"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
@@ -3419,9 +3460,15 @@
       <c r="I42" s="32"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="32"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
@@ -3444,55 +3491,140 @@
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C48" s="39"/>
+      <c r="A48" s="4"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="39"/>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="37"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="37"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F51" s="29"/>
-      <c r="G51" s="25"/>
-    </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-    </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-    </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-    </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-    </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-    </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="68"/>
+      <c r="D51" s="68"/>
+      <c r="E51" s="68"/>
+      <c r="F51" s="68"/>
+      <c r="G51" s="68"/>
+      <c r="H51" s="68"/>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" s="68"/>
+      <c r="D52" s="68"/>
+      <c r="E52" s="68"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="68"/>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="68"/>
+      <c r="D53" s="68"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="68"/>
+      <c r="G53" s="68"/>
+      <c r="H53" s="68"/>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="68"/>
+      <c r="D54" s="68"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="68"/>
+      <c r="G54" s="68"/>
+      <c r="H54" s="68"/>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" s="68"/>
+      <c r="D55" s="68"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="68"/>
+      <c r="G55" s="68"/>
+      <c r="H55" s="68"/>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56" s="68"/>
+      <c r="D56" s="68"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="68"/>
+      <c r="G56" s="68"/>
+      <c r="H56" s="68"/>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="68"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="69"/>
+      <c r="G57" s="69"/>
+      <c r="H57" s="68"/>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C58" s="68"/>
+      <c r="D58" s="68"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="68"/>
+      <c r="G58" s="68"/>
+      <c r="H58" s="68"/>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C59" s="68"/>
+      <c r="D59" s="68"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="68"/>
+      <c r="G59" s="68"/>
+      <c r="H59" s="68"/>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C60" s="68"/>
+      <c r="D60" s="68"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="69"/>
+      <c r="G60" s="69"/>
+      <c r="H60" s="68"/>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C61" s="68"/>
+      <c r="D61" s="68"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="69"/>
+      <c r="G61" s="69"/>
+      <c r="H61" s="68"/>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C62" s="68"/>
+      <c r="D62" s="68"/>
+      <c r="E62" s="68"/>
+      <c r="F62" s="69"/>
+      <c r="G62" s="69"/>
+      <c r="H62" s="68"/>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C63" s="68"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="68"/>
+      <c r="F63" s="69"/>
+      <c r="G63" s="69"/>
+      <c r="H63" s="68"/>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C64" s="68"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="68"/>
+      <c r="F64" s="69"/>
+      <c r="G64" s="69"/>
+      <c r="H64" s="68"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I2" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A2:I2"/>
   <mergeCells count="5">
     <mergeCell ref="H5:H7"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="I5:I7"/>
-    <mergeCell ref="H37:H40"/>
+    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>